<commit_message>
Turbsim-files nur bei Bedarf erzeugen
</commit_message>
<xml_diff>
--- a/Matlab/openFAST_config.xlsx
+++ b/Matlab/openFAST_config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -101,16 +101,16 @@
     <t xml:space="preserve">1p1</t>
   </si>
   <si>
+    <t xml:space="preserve">[10 15 20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p1_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">NTM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[10 15 20]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1p1_2</t>
   </si>
   <si>
     <t xml:space="preserve">[12 14]</t>
@@ -346,7 +346,7 @@
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.22"/>
@@ -436,10 +436,10 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.55"/>
@@ -489,22 +489,19 @@
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Switch ersetzt; files als struct
</commit_message>
<xml_diff>
--- a/Matlab/openFAST_config.xlsx
+++ b/Matlab/openFAST_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -29,43 +29,49 @@
     <t xml:space="preserve">MainInput</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_preproc/sim/5MW_Land_DLL_WTurb.fst</t>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/5MW_Land_DLL_WTurb.fst</t>
   </si>
   <si>
     <t xml:space="preserve">ElastoDyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_preproc/sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_Onshore_ElastoDyn.dat</t>
   </si>
   <si>
     <t xml:space="preserve">ServoDyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_preproc/sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_Onshore_ServoDyn.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Aerodyn</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_preproc/sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_Onshore_AeroDyn15.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Inflowind</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_preproc/sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim/NRELOffshrBsline5MW_InflowWind_12mps.dat</t>
   </si>
   <si>
     <t xml:space="preserve">Turbsim</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_preproc/wind/TurbSim.inp</t>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/wind/TurbSim.inp</t>
   </si>
   <si>
     <t xml:space="preserve">Simulation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/ohel/Schreibtisch/FAST_preproc</t>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/sim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/hannah/Schreibtisch/openFAST_preproc/wind</t>
   </si>
   <si>
     <t xml:space="preserve">DLC Group</t>
@@ -107,6 +113,9 @@
     <t xml:space="preserve">1p1</t>
   </si>
   <si>
+    <t xml:space="preserve">NTM</t>
+  </si>
+  <si>
     <t xml:space="preserve">[10 15 20]</t>
   </si>
   <si>
@@ -120,9 +129,6 @@
   </si>
   <si>
     <t xml:space="preserve">1p1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTM</t>
   </si>
   <si>
     <t xml:space="preserve">[12 14]</t>
@@ -151,7 +157,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -180,6 +186,14 @@
       <color rgb="FF000000"/>
       <name val="CMU Sans Serif"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="CMU Sans Serif"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -245,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -255,6 +269,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -355,10 +377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,47 +395,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -424,12 +446,20 @@
     <row r="8" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -450,18 +480,18 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="1.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.55"/>
@@ -470,94 +500,97 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="11.55"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="6" t="s">
+    <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="K1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
+      <c r="E3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>